<commit_message>
Flujo completo de consulta Venta Tipo 1
</commit_message>
<xml_diff>
--- a/resources/insumoEbindLATAM.xlsx
+++ b/resources/insumoEbindLATAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21D514C-A5E4-4F9A-BC9D-F5E3EBC9029B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720CE325-1221-4A70-8807-9357204F4047}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{9868DF3B-556E-4CB5-9D37-E33C6EFC3E5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t>AFILIACION</t>
   </si>
@@ -204,10 +204,6 @@
     <t>20230727</t>
   </si>
   <si>
-    <t xml:space="preserve">
-72715812158100155801294</t>
-  </si>
-  <si>
     <t>000000204068</t>
   </si>
   <si>
@@ -238,7 +234,43 @@
     <t>21577420041218</t>
   </si>
   <si>
-    <t>00110197009500000057</t>
+    <t>00110197009500000058</t>
+  </si>
+  <si>
+    <t>001108140100012109</t>
+  </si>
+  <si>
+    <t>72715812158100155801294</t>
+  </si>
+  <si>
+    <t>216545412212</t>
+  </si>
+  <si>
+    <t>476173******0119</t>
+  </si>
+  <si>
+    <t>74745702158100100300197</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>21577270040904</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Débito</t>
+  </si>
+  <si>
+    <t>00111999009500000044</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>001108140100012141</t>
   </si>
 </sst>
 </file>
@@ -380,7 +412,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,6 +425,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F157F-1554-4AB2-83B6-9BC465217A6B}">
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,12 +875,12 @@
         <v>21</v>
       </c>
       <c r="AF1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>2</v>
@@ -860,26 +894,26 @@
       <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="15">
+      <c r="F2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="14">
         <v>0.88249999999999995</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>60</v>
+      <c r="I2" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="19" t="s">
-        <v>59</v>
+      <c r="L2" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>14</v>
@@ -887,14 +921,14 @@
       <c r="N2" s="10">
         <v>597.59</v>
       </c>
-      <c r="O2" s="17" t="s">
-        <v>68</v>
+      <c r="O2" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="P2" s="10">
         <v>604</v>
       </c>
-      <c r="Q2" s="17" t="s">
-        <v>69</v>
+      <c r="Q2" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="R2" t="s">
         <v>50</v>
@@ -908,23 +942,23 @@
       <c r="U2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="V2" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="W2" s="12">
-        <v>1108140100012100</v>
-      </c>
-      <c r="X2" s="16" t="s">
-        <v>61</v>
+      <c r="X2" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
-      <c r="Z2" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA2" s="16" t="s">
-        <v>62</v>
+      <c r="Z2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="AB2" s="10" t="s">
         <v>52</v>
@@ -944,26 +978,91 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0.57434027777777774</v>
+      </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="9"/>
+      <c r="K3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>74</v>
+      </c>
       <c r="M3" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="P3" s="10">
+        <v>604</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="S3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="V3" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y3" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="AD3" s="8" t="s">
         <v>20</v>
@@ -977,7 +1076,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -1012,7 +1111,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -1020,7 +1119,7 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="14"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="11"/>
       <c r="H5" s="1" t="s">
         <v>12</v>
@@ -1046,7 +1145,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -1054,7 +1153,7 @@
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="14"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="11"/>
       <c r="H6" s="1" t="s">
         <v>13</v>
@@ -1091,15 +1190,20 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="E8" s="3"/>
-      <c r="F8" s="18">
-        <v>44718</v>
-      </c>
+      <c r="F8" s="17"/>
       <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="3"/>
+      <c r="W10" s="3"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feature que soluciona variantes de detalle de venta de 26 y 30 campos
</commit_message>
<xml_diff>
--- a/resources/insumoEbindLATAM.xlsx
+++ b/resources/insumoEbindLATAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720CE325-1221-4A70-8807-9357204F4047}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5598E574-CB45-4A72-A850-E8101D82C9CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{9868DF3B-556E-4CB5-9D37-E33C6EFC3E5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>AFILIACION</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>001108140100012141</t>
+  </si>
+  <si>
+    <t>Importe Propina</t>
   </si>
 </sst>
 </file>
@@ -745,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F157F-1554-4AB2-83B6-9BC465217A6B}">
-  <dimension ref="A1:AF21"/>
+  <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,11 +779,12 @@
     <col min="27" max="27" width="20.26953125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="21.7265625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="24.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.54296875" customWidth="1"/>
-    <col min="32" max="32" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.36328125" customWidth="1"/>
+    <col min="31" max="31" width="15.54296875" customWidth="1"/>
+    <col min="33" max="33" width="19.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -869,16 +873,19 @@
         <v>43</v>
       </c>
       <c r="AD1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE1" t="s">
         <v>19</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>63</v>
       </c>
@@ -966,17 +973,18 @@
       <c r="AC2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>8584</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
@@ -1064,17 +1072,18 @@
       <c r="AC3" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="3">
         <v>8797</v>
       </c>
-      <c r="AF3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" ht="25" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>64</v>
       </c>
@@ -1084,7 +1093,7 @@
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="11"/>
       <c r="H4" s="1" t="s">
         <v>11</v>
@@ -1094,22 +1103,29 @@
         <v>6</v>
       </c>
       <c r="K4" s="9"/>
-      <c r="L4" s="5"/>
       <c r="M4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="Q4" s="3"/>
-      <c r="AD4" s="8" t="s">
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>15059</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" ht="25" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>63</v>
       </c>
@@ -1132,18 +1148,25 @@
       <c r="M5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="V5" s="3"/>
-      <c r="AD5" s="8" t="s">
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>8958</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
@@ -1166,17 +1189,20 @@
       <c r="M6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AD6" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AE6" s="3">
+      <c r="AF6" s="3">
         <v>16348</v>
       </c>
-      <c r="AF6" s="4" t="s">
+      <c r="AG6" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="D7" s="5"/>
@@ -1187,20 +1213,30 @@
       <c r="V7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AD7" s="5"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="E8" s="3"/>
       <c r="F8" s="17"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="E10" s="5"/>
       <c r="F10" s="3"/>
       <c r="W10" s="3"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AH11" s="3"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="C14" s="3"/>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E21" s="3"/>

</xml_diff>

<commit_message>
Correcion a metodo que busca en el front para que acepte cualquier longitud y validacion de sesiones abiertas
</commit_message>
<xml_diff>
--- a/resources/insumoEbindLATAM.xlsx
+++ b/resources/insumoEbindLATAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5598E574-CB45-4A72-A850-E8101D82C9CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B5DE0D-C6FD-4D34-83E2-2545A155047F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{9868DF3B-556E-4CB5-9D37-E33C6EFC3E5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
   <si>
     <t>AFILIACION</t>
   </si>
@@ -243,37 +243,43 @@
     <t>72715812158100155801294</t>
   </si>
   <si>
+    <t>476173******0119</t>
+  </si>
+  <si>
+    <t>74745702158100100300197</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>21577270040904</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Débito</t>
+  </si>
+  <si>
+    <t>00111999009500000044</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>001108140100012141</t>
+  </si>
+  <si>
+    <t>Importe Propina</t>
+  </si>
+  <si>
+    <t>FECHA I</t>
+  </si>
+  <si>
+    <t>FECHA F</t>
+  </si>
+  <si>
     <t>216545412212</t>
-  </si>
-  <si>
-    <t>476173******0119</t>
-  </si>
-  <si>
-    <t>74745702158100100300197</t>
-  </si>
-  <si>
-    <t>10.00</t>
-  </si>
-  <si>
-    <t>21577270040904</t>
-  </si>
-  <si>
-    <t>Visa</t>
-  </si>
-  <si>
-    <t>Débito</t>
-  </si>
-  <si>
-    <t>00111999009500000044</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>001108140100012141</t>
-  </si>
-  <si>
-    <t>Importe Propina</t>
   </si>
 </sst>
 </file>
@@ -388,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -433,6 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F157F-1554-4AB2-83B6-9BC465217A6B}">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AI21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -784,7 +791,7 @@
     <col min="33" max="33" width="19.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -873,7 +880,7 @@
         <v>43</v>
       </c>
       <c r="AD1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE1" t="s">
         <v>19</v>
@@ -884,8 +891,14 @@
       <c r="AG1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AH1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>63</v>
       </c>
@@ -983,8 +996,14 @@
       <c r="AG2" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AH2" s="20">
+        <v>45078</v>
+      </c>
+      <c r="AI2" s="20">
+        <v>45137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
@@ -1010,22 +1029,22 @@
         <v>10</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="18" t="s">
         <v>73</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>74</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O3" s="16" t="s">
         <v>67</v>
@@ -1034,10 +1053,10 @@
         <v>604</v>
       </c>
       <c r="Q3" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="S3" t="s">
         <v>51</v>
@@ -1046,19 +1065,19 @@
         <v>51</v>
       </c>
       <c r="U3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="V3" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="V3" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="W3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X3" s="15" t="s">
         <v>60</v>
       </c>
       <c r="Y3" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z3" s="15" t="s">
         <v>61</v>
@@ -1083,7 +1102,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>64</v>
       </c>
@@ -1125,7 +1144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>63</v>
       </c>
@@ -1166,7 +1185,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
@@ -1202,7 +1221,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="D7" s="5"/>
@@ -1215,28 +1234,34 @@
       <c r="AC7" s="5"/>
       <c r="AD7" s="5"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="E8" s="3"/>
       <c r="F8" s="17"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="E10" s="5"/>
       <c r="F10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="AH11" s="3"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="C12" s="3"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="W16" s="3"/>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E21" s="3"/>

</xml_diff>

<commit_message>
EntregaFinal Version 1 Latam
</commit_message>
<xml_diff>
--- a/resources/insumoEbindLATAM.xlsx
+++ b/resources/insumoEbindLATAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B5DE0D-C6FD-4D34-83E2-2545A155047F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E3FCF9-2A04-4066-920D-6F3A97CE33CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{9868DF3B-556E-4CB5-9D37-E33C6EFC3E5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
   <si>
     <t>AFILIACION</t>
   </si>
@@ -273,13 +273,19 @@
     <t>Importe Propina</t>
   </si>
   <si>
-    <t>FECHA I</t>
-  </si>
-  <si>
-    <t>FECHA F</t>
-  </si>
-  <si>
     <t>216545412212</t>
+  </si>
+  <si>
+    <t>Fecha I</t>
+  </si>
+  <si>
+    <t>Fecha F</t>
+  </si>
+  <si>
+    <t>20230601</t>
+  </si>
+  <si>
+    <t>20230701</t>
   </si>
 </sst>
 </file>
@@ -394,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -439,7 +445,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F157F-1554-4AB2-83B6-9BC465217A6B}">
-  <dimension ref="A1:AI21"/>
+  <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC19" activeCellId="1" sqref="AB26 AC19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -892,10 +897,10 @@
         <v>62</v>
       </c>
       <c r="AH1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.35">
@@ -996,11 +1001,11 @@
       <c r="AG2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="20">
-        <v>45078</v>
-      </c>
-      <c r="AI2" s="20">
-        <v>45137</v>
+      <c r="AH2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
@@ -1029,7 +1034,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
@@ -1254,6 +1259,9 @@
     <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="C12" s="3"/>
     </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AA13" s="3"/>
+    </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="C14" s="3"/>
     </row>
@@ -1263,8 +1271,20 @@
     <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="W16" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:32" x14ac:dyDescent="0.35">
+      <c r="AF18" s="3"/>
+    </row>
+    <row r="19" spans="5:32" x14ac:dyDescent="0.35">
+      <c r="AA19" s="5"/>
+    </row>
+    <row r="20" spans="5:32" x14ac:dyDescent="0.35">
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="5:32" x14ac:dyDescent="0.35">
       <c r="E21" s="3"/>
+    </row>
+    <row r="26" spans="5:32" x14ac:dyDescent="0.35">
+      <c r="AB26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
últimos cambios durante reunion viernes Hugo
</commit_message>
<xml_diff>
--- a/resources/insumoEbindLATAM.xlsx
+++ b/resources/insumoEbindLATAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E3FCF9-2A04-4066-920D-6F3A97CE33CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82C00D5-140F-4BD9-9277-D85729D4F36D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{9868DF3B-556E-4CB5-9D37-E33C6EFC3E5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
   <si>
     <t>AFILIACION</t>
   </si>
@@ -274,18 +274,6 @@
   </si>
   <si>
     <t>216545412212</t>
-  </si>
-  <si>
-    <t>Fecha I</t>
-  </si>
-  <si>
-    <t>Fecha F</t>
-  </si>
-  <si>
-    <t>20230601</t>
-  </si>
-  <si>
-    <t>20230701</t>
   </si>
 </sst>
 </file>
@@ -762,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F157F-1554-4AB2-83B6-9BC465217A6B}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC19" activeCellId="1" sqref="AB26 AC19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -896,12 +884,6 @@
       <c r="AG1" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -1001,12 +983,8 @@
       <c r="AG2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1282,6 +1260,7 @@
     </row>
     <row r="21" spans="5:32" x14ac:dyDescent="0.35">
       <c r="E21" s="3"/>
+      <c r="AE21" s="3"/>
     </row>
     <row r="26" spans="5:32" x14ac:dyDescent="0.35">
       <c r="AB26" s="3"/>

</xml_diff>

<commit_message>
Venta por fechas y validaciones
</commit_message>
<xml_diff>
--- a/resources/insumoEbindLATAM.xlsx
+++ b/resources/insumoEbindLATAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icf2303\Documents\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82C00D5-140F-4BD9-9277-D85729D4F36D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332AF391-5DEF-40E8-8775-72E10CF9CFC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{9868DF3B-556E-4CB5-9D37-E33C6EFC3E5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t>AFILIACION</t>
   </si>
@@ -213,9 +213,6 @@
     <t>00</t>
   </si>
   <si>
-    <t>Fecha proceso ListBox</t>
-  </si>
-  <si>
     <t>07-06-2023</t>
   </si>
   <si>
@@ -274,6 +271,15 @@
   </si>
   <si>
     <t>216545412212</t>
+  </si>
+  <si>
+    <t>Fecha Inicial</t>
+  </si>
+  <si>
+    <t>Fecha Final</t>
+  </si>
+  <si>
+    <t>202307277</t>
   </si>
 </sst>
 </file>
@@ -750,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F157F-1554-4AB2-83B6-9BC465217A6B}">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V21" sqref="V20:V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -873,7 +879,7 @@
         <v>43</v>
       </c>
       <c r="AD1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AE1" t="s">
         <v>19</v>
@@ -882,12 +888,15 @@
         <v>21</v>
       </c>
       <c r="AG1" t="s">
-        <v>62</v>
+        <v>82</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>2</v>
@@ -902,7 +911,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="14">
         <v>0.88249999999999995</v>
@@ -920,7 +929,7 @@
         <v>49</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>14</v>
@@ -929,13 +938,13 @@
         <v>597.59</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P2" s="10">
         <v>604</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R2" t="s">
         <v>50</v>
@@ -950,10 +959,10 @@
         <v>54</v>
       </c>
       <c r="V2" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="W2" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="X2" s="15" t="s">
         <v>60</v>
@@ -983,12 +992,14 @@
       <c r="AG2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="4"/>
+      <c r="AH2" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="AI2" s="4"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>2</v>
@@ -1003,7 +1014,7 @@
         <v>48</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="14">
         <v>0.57434027777777774</v>
@@ -1012,34 +1023,34 @@
         <v>10</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="18" t="s">
         <v>72</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>73</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P3" s="10">
         <v>604</v>
       </c>
       <c r="Q3" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="S3" t="s">
         <v>51</v>
@@ -1048,19 +1059,19 @@
         <v>51</v>
       </c>
       <c r="U3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="V3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="V3" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="W3" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X3" s="15" t="s">
         <v>60</v>
       </c>
       <c r="Y3" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Z3" s="15" t="s">
         <v>61</v>
@@ -1084,10 +1095,13 @@
       <c r="AG3" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="AH3" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -1126,10 +1140,13 @@
       <c r="AG4" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="AH4" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
@@ -1167,10 +1184,13 @@
       <c r="AG5" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AH5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="25" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>2</v>
@@ -1192,7 +1212,7 @@
         <v>18</v>
       </c>
       <c r="AD6" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE6" s="8" t="s">
         <v>20</v>
@@ -1201,6 +1221,9 @@
         <v>16348</v>
       </c>
       <c r="AG6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH6" s="1" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>